<commit_message>
Initial commit 03-12-2025  1:26:53.03
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i5 GAMING\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E7BD39C5-1884-4840-9645-10B01024AEF6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEDAE9A-2C39-493A-B109-07994DC6E82F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mock Test 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="638">
   <si>
     <t>Sl No</t>
   </si>
@@ -2792,6 +2792,45 @@
   </si>
   <si>
     <t>All of the above</t>
+  </si>
+  <si>
+    <t>Subjects Covered</t>
+  </si>
+  <si>
+    <t>Time in Minute/Question</t>
+  </si>
+  <si>
+    <t>General Knowledge</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Civics</t>
+  </si>
+  <si>
+    <t>Indian Constitution</t>
+  </si>
+  <si>
+    <t>Arts, Literature, Culture, Sports</t>
+  </si>
+  <si>
+    <t>Basic of Computer</t>
+  </si>
+  <si>
+    <t>Science and Technology</t>
+  </si>
+  <si>
+    <t>Simple Arithmetic, Mental Ability and Reasoning</t>
+  </si>
+  <si>
+    <t>General English</t>
+  </si>
+  <si>
+    <t>Regional Language (Malayalam)</t>
   </si>
 </sst>
 </file>
@@ -3170,20 +3209,20 @@
   </sheetPr>
   <dimension ref="A1:AK999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="4" width="12.5703125" style="13"/>
-    <col min="5" max="5" width="40.140625" style="13" customWidth="1"/>
-    <col min="6" max="11" width="12.5703125" style="13"/>
-    <col min="12" max="12" width="47.5703125" style="13" customWidth="1"/>
-    <col min="13" max="16384" width="12.5703125" style="13"/>
+    <col min="1" max="4" width="12.54296875" style="13"/>
+    <col min="5" max="5" width="40.1796875" style="13" customWidth="1"/>
+    <col min="6" max="11" width="12.54296875" style="13"/>
+    <col min="12" max="12" width="47.54296875" style="13" customWidth="1"/>
+    <col min="13" max="16384" width="12.54296875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="51">
+    <row r="1" spans="1:37" ht="52">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3268,8 +3307,14 @@
       <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" ht="331.5">
+      <c r="AC1" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="287.5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3330,8 +3375,12 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
+      <c r="AC2" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0.75</v>
+      </c>
       <c r="AE2" s="14"/>
       <c r="AF2" s="14"/>
       <c r="AG2" s="14"/>
@@ -3340,7 +3389,7 @@
       <c r="AJ2" s="14"/>
       <c r="AK2" s="14"/>
     </row>
-    <row r="3" spans="1:37" ht="344.25">
+    <row r="3" spans="1:37" ht="337.5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3401,8 +3450,10 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
+      <c r="AC3" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="AD3" s="2"/>
       <c r="AE3" s="14"/>
       <c r="AF3" s="14"/>
       <c r="AG3" s="14"/>
@@ -3474,8 +3525,10 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
+      <c r="AC4" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="AD4" s="2"/>
       <c r="AE4" s="14"/>
       <c r="AF4" s="14"/>
       <c r="AG4" s="14"/>
@@ -3484,7 +3537,7 @@
       <c r="AJ4" s="14"/>
       <c r="AK4" s="14"/>
     </row>
-    <row r="5" spans="1:37" ht="344.25">
+    <row r="5" spans="1:37" ht="325">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3545,8 +3598,10 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
+      <c r="AC5" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="AD5" s="2"/>
       <c r="AE5" s="14"/>
       <c r="AF5" s="14"/>
       <c r="AG5" s="14"/>
@@ -3616,8 +3671,10 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
+      <c r="AC6" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="AD6" s="2"/>
       <c r="AE6" s="14"/>
       <c r="AF6" s="14"/>
       <c r="AG6" s="14"/>
@@ -3626,7 +3683,7 @@
       <c r="AJ6" s="14"/>
       <c r="AK6" s="14"/>
     </row>
-    <row r="7" spans="1:37" ht="216.75">
+    <row r="7" spans="1:37" ht="200">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3687,8 +3744,10 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
+      <c r="AC7" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD7" s="2"/>
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14"/>
@@ -3697,7 +3756,7 @@
       <c r="AJ7" s="14"/>
       <c r="AK7" s="14"/>
     </row>
-    <row r="8" spans="1:37" ht="409.5">
+    <row r="8" spans="1:37" ht="387.5">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3758,8 +3817,10 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
+      <c r="AC8" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="AD8" s="2"/>
       <c r="AE8" s="14"/>
       <c r="AF8" s="14"/>
       <c r="AG8" s="14"/>
@@ -3829,8 +3890,10 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
+      <c r="AC9" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="AD9" s="2"/>
       <c r="AE9" s="14"/>
       <c r="AF9" s="14"/>
       <c r="AG9" s="14"/>
@@ -3839,7 +3902,7 @@
       <c r="AJ9" s="14"/>
       <c r="AK9" s="14"/>
     </row>
-    <row r="10" spans="1:37" ht="153">
+    <row r="10" spans="1:37" ht="150">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3900,8 +3963,10 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
+      <c r="AC10" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="AD10" s="2"/>
       <c r="AE10" s="14"/>
       <c r="AF10" s="14"/>
       <c r="AG10" s="14"/>
@@ -3973,8 +4038,10 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
+      <c r="AC11" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="AD11" s="2"/>
       <c r="AE11" s="14"/>
       <c r="AF11" s="14"/>
       <c r="AG11" s="14"/>
@@ -4038,8 +4105,10 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
+      <c r="AC12" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="AD12" s="2"/>
       <c r="AE12" s="14"/>
       <c r="AF12" s="14"/>
       <c r="AG12" s="14"/>
@@ -4099,8 +4168,8 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
       <c r="AE13" s="15"/>
       <c r="AF13" s="15"/>
       <c r="AG13" s="15"/>
@@ -4160,8 +4229,10 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="16"/>
       <c r="AB14" s="16"/>
-    </row>
-    <row r="15" spans="1:37" ht="369.75">
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="16"/>
+    </row>
+    <row r="15" spans="1:37" ht="350">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4210,8 +4281,10 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="16"/>
       <c r="AB15" s="16"/>
-    </row>
-    <row r="16" spans="1:37" ht="369.75">
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+    </row>
+    <row r="16" spans="1:37" ht="350">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4260,8 +4333,10 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="16"/>
       <c r="AB16" s="16"/>
-    </row>
-    <row r="17" spans="1:28" ht="395.25">
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+    </row>
+    <row r="17" spans="1:30" ht="375">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4310,8 +4385,10 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="16"/>
       <c r="AB17" s="16"/>
-    </row>
-    <row r="18" spans="1:28" ht="409.5">
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16"/>
+    </row>
+    <row r="18" spans="1:30" ht="409.5">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -4360,8 +4437,10 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="16"/>
       <c r="AB18" s="16"/>
-    </row>
-    <row r="19" spans="1:28" ht="409.5">
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="16"/>
+    </row>
+    <row r="19" spans="1:30" ht="409.5">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4410,8 +4489,10 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="16"/>
       <c r="AB19" s="16"/>
-    </row>
-    <row r="20" spans="1:28" ht="409.5">
+      <c r="AC19" s="16"/>
+      <c r="AD19" s="16"/>
+    </row>
+    <row r="20" spans="1:30" ht="409.5">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4460,8 +4541,10 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="16"/>
       <c r="AB20" s="16"/>
-    </row>
-    <row r="21" spans="1:28" ht="409.5">
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+    </row>
+    <row r="21" spans="1:30" ht="409.5">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4510,8 +4593,10 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="16"/>
       <c r="AB21" s="16"/>
-    </row>
-    <row r="22" spans="1:28" ht="409.5">
+      <c r="AC21" s="16"/>
+      <c r="AD21" s="16"/>
+    </row>
+    <row r="22" spans="1:30" ht="409.5">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -4560,8 +4645,10 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="16"/>
       <c r="AB22" s="16"/>
-    </row>
-    <row r="23" spans="1:28" ht="409.5">
+      <c r="AC22" s="16"/>
+      <c r="AD22" s="16"/>
+    </row>
+    <row r="23" spans="1:30" ht="409.5">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -4610,8 +4697,10 @@
       <c r="Z23" s="16"/>
       <c r="AA23" s="16"/>
       <c r="AB23" s="16"/>
-    </row>
-    <row r="24" spans="1:28" ht="409.5">
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
+    </row>
+    <row r="24" spans="1:30" ht="409.5">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -4660,8 +4749,10 @@
       <c r="Z24" s="16"/>
       <c r="AA24" s="16"/>
       <c r="AB24" s="16"/>
-    </row>
-    <row r="25" spans="1:28" ht="409.5">
+      <c r="AC24" s="16"/>
+      <c r="AD24" s="16"/>
+    </row>
+    <row r="25" spans="1:30" ht="409.5">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -4710,8 +4801,10 @@
       <c r="Z25" s="16"/>
       <c r="AA25" s="16"/>
       <c r="AB25" s="16"/>
-    </row>
-    <row r="26" spans="1:28" ht="409.5">
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="16"/>
+    </row>
+    <row r="26" spans="1:30" ht="375">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -4760,8 +4853,10 @@
       <c r="Z26" s="16"/>
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
-    </row>
-    <row r="27" spans="1:28" ht="395.25">
+      <c r="AC26" s="16"/>
+      <c r="AD26" s="16"/>
+    </row>
+    <row r="27" spans="1:30" ht="350">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4810,8 +4905,10 @@
       <c r="Z27" s="16"/>
       <c r="AA27" s="16"/>
       <c r="AB27" s="16"/>
-    </row>
-    <row r="28" spans="1:28" ht="409.5">
+      <c r="AC27" s="16"/>
+      <c r="AD27" s="16"/>
+    </row>
+    <row r="28" spans="1:30" ht="409.5">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -4860,8 +4957,10 @@
       <c r="Z28" s="16"/>
       <c r="AA28" s="16"/>
       <c r="AB28" s="16"/>
-    </row>
-    <row r="29" spans="1:28" ht="409.5">
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="16"/>
+    </row>
+    <row r="29" spans="1:30" ht="409.5">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -4910,8 +5009,10 @@
       <c r="Z29" s="16"/>
       <c r="AA29" s="16"/>
       <c r="AB29" s="16"/>
-    </row>
-    <row r="30" spans="1:28" ht="409.5">
+      <c r="AC29" s="16"/>
+      <c r="AD29" s="16"/>
+    </row>
+    <row r="30" spans="1:30" ht="409.5">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -4960,8 +5061,10 @@
       <c r="Z30" s="16"/>
       <c r="AA30" s="16"/>
       <c r="AB30" s="16"/>
-    </row>
-    <row r="31" spans="1:28" ht="409.5">
+      <c r="AC30" s="16"/>
+      <c r="AD30" s="16"/>
+    </row>
+    <row r="31" spans="1:30" ht="409.5">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5010,8 +5113,10 @@
       <c r="Z31" s="16"/>
       <c r="AA31" s="16"/>
       <c r="AB31" s="16"/>
-    </row>
-    <row r="32" spans="1:28" ht="409.5">
+      <c r="AC31" s="16"/>
+      <c r="AD31" s="16"/>
+    </row>
+    <row r="32" spans="1:30" ht="409.5">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5060,8 +5165,10 @@
       <c r="Z32" s="16"/>
       <c r="AA32" s="16"/>
       <c r="AB32" s="16"/>
-    </row>
-    <row r="33" spans="1:28" ht="409.5">
+      <c r="AC32" s="16"/>
+      <c r="AD32" s="16"/>
+    </row>
+    <row r="33" spans="1:30" ht="409.5">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5110,8 +5217,10 @@
       <c r="Z33" s="16"/>
       <c r="AA33" s="16"/>
       <c r="AB33" s="16"/>
-    </row>
-    <row r="34" spans="1:28" ht="306">
+      <c r="AC33" s="16"/>
+      <c r="AD33" s="16"/>
+    </row>
+    <row r="34" spans="1:30" ht="300">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5160,8 +5269,10 @@
       <c r="Z34" s="16"/>
       <c r="AA34" s="16"/>
       <c r="AB34" s="16"/>
-    </row>
-    <row r="35" spans="1:28" ht="178.5">
+      <c r="AC34" s="16"/>
+      <c r="AD34" s="16"/>
+    </row>
+    <row r="35" spans="1:30" ht="175">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5210,8 +5321,10 @@
       <c r="Z35" s="16"/>
       <c r="AA35" s="16"/>
       <c r="AB35" s="16"/>
-    </row>
-    <row r="36" spans="1:28" ht="318.75">
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+    </row>
+    <row r="36" spans="1:30" ht="312.5">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5260,8 +5373,10 @@
       <c r="Z36" s="16"/>
       <c r="AA36" s="16"/>
       <c r="AB36" s="16"/>
-    </row>
-    <row r="37" spans="1:28" ht="242.25">
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="16"/>
+    </row>
+    <row r="37" spans="1:30" ht="237.5">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5310,8 +5425,10 @@
       <c r="Z37" s="16"/>
       <c r="AA37" s="16"/>
       <c r="AB37" s="16"/>
-    </row>
-    <row r="38" spans="1:28" ht="140.25">
+      <c r="AC37" s="16"/>
+      <c r="AD37" s="16"/>
+    </row>
+    <row r="38" spans="1:30" ht="137.5">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5360,8 +5477,10 @@
       <c r="Z38" s="16"/>
       <c r="AA38" s="16"/>
       <c r="AB38" s="16"/>
-    </row>
-    <row r="39" spans="1:28" ht="255">
+      <c r="AC38" s="16"/>
+      <c r="AD38" s="16"/>
+    </row>
+    <row r="39" spans="1:30" ht="237.5">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5410,8 +5529,10 @@
       <c r="Z39" s="16"/>
       <c r="AA39" s="16"/>
       <c r="AB39" s="16"/>
-    </row>
-    <row r="40" spans="1:28" ht="255">
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="16"/>
+    </row>
+    <row r="40" spans="1:30" ht="225">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5460,8 +5581,10 @@
       <c r="Z40" s="16"/>
       <c r="AA40" s="16"/>
       <c r="AB40" s="16"/>
-    </row>
-    <row r="41" spans="1:28" ht="153">
+      <c r="AC40" s="16"/>
+      <c r="AD40" s="16"/>
+    </row>
+    <row r="41" spans="1:30" ht="150">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5510,8 +5633,10 @@
       <c r="Z41" s="16"/>
       <c r="AA41" s="16"/>
       <c r="AB41" s="16"/>
-    </row>
-    <row r="42" spans="1:28" ht="357">
+      <c r="AC41" s="16"/>
+      <c r="AD41" s="16"/>
+    </row>
+    <row r="42" spans="1:30" ht="337.5">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -5560,8 +5685,10 @@
       <c r="Z42" s="16"/>
       <c r="AA42" s="16"/>
       <c r="AB42" s="16"/>
-    </row>
-    <row r="43" spans="1:28" ht="165.75">
+      <c r="AC42" s="16"/>
+      <c r="AD42" s="16"/>
+    </row>
+    <row r="43" spans="1:30" ht="150">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5610,8 +5737,10 @@
       <c r="Z43" s="16"/>
       <c r="AA43" s="16"/>
       <c r="AB43" s="16"/>
-    </row>
-    <row r="44" spans="1:28" ht="369.75">
+      <c r="AC43" s="16"/>
+      <c r="AD43" s="16"/>
+    </row>
+    <row r="44" spans="1:30" ht="350">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -5660,8 +5789,10 @@
       <c r="Z44" s="16"/>
       <c r="AA44" s="16"/>
       <c r="AB44" s="16"/>
-    </row>
-    <row r="45" spans="1:28" ht="267.75">
+      <c r="AC44" s="16"/>
+      <c r="AD44" s="16"/>
+    </row>
+    <row r="45" spans="1:30" ht="262.5">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5710,8 +5841,10 @@
       <c r="Z45" s="16"/>
       <c r="AA45" s="16"/>
       <c r="AB45" s="16"/>
-    </row>
-    <row r="46" spans="1:28" ht="191.25">
+      <c r="AC45" s="16"/>
+      <c r="AD45" s="16"/>
+    </row>
+    <row r="46" spans="1:30" ht="187.5">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -5760,8 +5893,10 @@
       <c r="Z46" s="16"/>
       <c r="AA46" s="16"/>
       <c r="AB46" s="16"/>
-    </row>
-    <row r="47" spans="1:28" ht="409.5">
+      <c r="AC46" s="16"/>
+      <c r="AD46" s="16"/>
+    </row>
+    <row r="47" spans="1:30" ht="409.5">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -5810,8 +5945,10 @@
       <c r="Z47" s="16"/>
       <c r="AA47" s="16"/>
       <c r="AB47" s="16"/>
-    </row>
-    <row r="48" spans="1:28" ht="382.5">
+      <c r="AC47" s="16"/>
+      <c r="AD47" s="16"/>
+    </row>
+    <row r="48" spans="1:30" ht="375">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -5860,6 +5997,8 @@
       <c r="Z48" s="16"/>
       <c r="AA48" s="16"/>
       <c r="AB48" s="16"/>
+      <c r="AC48" s="16"/>
+      <c r="AD48" s="16"/>
     </row>
     <row r="49" spans="1:37" ht="409.5">
       <c r="A49" s="2">
@@ -5910,8 +6049,10 @@
       <c r="Z49" s="16"/>
       <c r="AA49" s="16"/>
       <c r="AB49" s="16"/>
-    </row>
-    <row r="50" spans="1:37" ht="331.5">
+      <c r="AC49" s="16"/>
+      <c r="AD49" s="16"/>
+    </row>
+    <row r="50" spans="1:37" ht="312.5">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -5960,6 +6101,8 @@
       <c r="Z50" s="16"/>
       <c r="AA50" s="16"/>
       <c r="AB50" s="16"/>
+      <c r="AC50" s="16"/>
+      <c r="AD50" s="16"/>
     </row>
     <row r="51" spans="1:37" ht="409.5">
       <c r="A51" s="2">
@@ -6010,8 +6153,10 @@
       <c r="Z51" s="16"/>
       <c r="AA51" s="16"/>
       <c r="AB51" s="16"/>
-    </row>
-    <row r="52" spans="1:37" ht="318.75">
+      <c r="AC51" s="16"/>
+      <c r="AD51" s="16"/>
+    </row>
+    <row r="52" spans="1:37" ht="300">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -6062,8 +6207,8 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
       <c r="AB52" s="5"/>
-      <c r="AC52" s="15"/>
-      <c r="AD52" s="15"/>
+      <c r="AC52" s="5"/>
+      <c r="AD52" s="5"/>
       <c r="AE52" s="15"/>
       <c r="AF52" s="15"/>
       <c r="AG52" s="15"/>
@@ -6072,7 +6217,7 @@
       <c r="AJ52" s="15"/>
       <c r="AK52" s="15"/>
     </row>
-    <row r="53" spans="1:37" ht="63.75">
+    <row r="53" spans="1:37" ht="50">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -6123,8 +6268,8 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AB53" s="5"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="15"/>
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="5"/>
       <c r="AE53" s="15"/>
       <c r="AF53" s="15"/>
       <c r="AG53" s="15"/>
@@ -6133,7 +6278,7 @@
       <c r="AJ53" s="15"/>
       <c r="AK53" s="15"/>
     </row>
-    <row r="54" spans="1:37" ht="76.5">
+    <row r="54" spans="1:37" ht="62.5">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -6184,8 +6329,8 @@
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
       <c r="AB54" s="5"/>
-      <c r="AC54" s="15"/>
-      <c r="AD54" s="15"/>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="5"/>
       <c r="AE54" s="15"/>
       <c r="AF54" s="15"/>
       <c r="AG54" s="15"/>
@@ -6194,7 +6339,7 @@
       <c r="AJ54" s="15"/>
       <c r="AK54" s="15"/>
     </row>
-    <row r="55" spans="1:37" ht="89.25">
+    <row r="55" spans="1:37" ht="75">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -6245,8 +6390,8 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
-      <c r="AC55" s="15"/>
-      <c r="AD55" s="15"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="5"/>
       <c r="AE55" s="15"/>
       <c r="AF55" s="15"/>
       <c r="AG55" s="15"/>
@@ -6255,7 +6400,7 @@
       <c r="AJ55" s="15"/>
       <c r="AK55" s="15"/>
     </row>
-    <row r="56" spans="1:37" ht="89.25">
+    <row r="56" spans="1:37" ht="87.5">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -6306,8 +6451,8 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
-      <c r="AC56" s="15"/>
-      <c r="AD56" s="15"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="5"/>
       <c r="AE56" s="15"/>
       <c r="AF56" s="15"/>
       <c r="AG56" s="15"/>
@@ -6316,7 +6461,7 @@
       <c r="AJ56" s="15"/>
       <c r="AK56" s="15"/>
     </row>
-    <row r="57" spans="1:37" ht="140.25">
+    <row r="57" spans="1:37" ht="137.5">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -6367,8 +6512,8 @@
       <c r="Z57" s="5"/>
       <c r="AA57" s="5"/>
       <c r="AB57" s="5"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="15"/>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="5"/>
       <c r="AE57" s="15"/>
       <c r="AF57" s="15"/>
       <c r="AG57" s="15"/>
@@ -6377,7 +6522,7 @@
       <c r="AJ57" s="15"/>
       <c r="AK57" s="15"/>
     </row>
-    <row r="58" spans="1:37" ht="178.5">
+    <row r="58" spans="1:37" ht="150">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -6428,8 +6573,8 @@
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
       <c r="AB58" s="5"/>
-      <c r="AC58" s="15"/>
-      <c r="AD58" s="15"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="5"/>
       <c r="AE58" s="15"/>
       <c r="AF58" s="15"/>
       <c r="AG58" s="15"/>
@@ -6438,7 +6583,7 @@
       <c r="AJ58" s="15"/>
       <c r="AK58" s="15"/>
     </row>
-    <row r="59" spans="1:37" ht="114.75">
+    <row r="59" spans="1:37" ht="100">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -6489,8 +6634,8 @@
       <c r="Z59" s="5"/>
       <c r="AA59" s="5"/>
       <c r="AB59" s="5"/>
-      <c r="AC59" s="15"/>
-      <c r="AD59" s="15"/>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="5"/>
       <c r="AE59" s="15"/>
       <c r="AF59" s="15"/>
       <c r="AG59" s="15"/>
@@ -6499,7 +6644,7 @@
       <c r="AJ59" s="15"/>
       <c r="AK59" s="15"/>
     </row>
-    <row r="60" spans="1:37" ht="76.5">
+    <row r="60" spans="1:37" ht="62.5">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -6550,8 +6695,8 @@
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
-      <c r="AC60" s="15"/>
-      <c r="AD60" s="15"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="5"/>
       <c r="AE60" s="15"/>
       <c r="AF60" s="15"/>
       <c r="AG60" s="15"/>
@@ -6560,7 +6705,7 @@
       <c r="AJ60" s="15"/>
       <c r="AK60" s="15"/>
     </row>
-    <row r="61" spans="1:37" ht="127.5">
+    <row r="61" spans="1:37" ht="125">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -6611,8 +6756,8 @@
       <c r="Z61" s="5"/>
       <c r="AA61" s="5"/>
       <c r="AB61" s="5"/>
-      <c r="AC61" s="15"/>
-      <c r="AD61" s="15"/>
+      <c r="AC61" s="5"/>
+      <c r="AD61" s="5"/>
       <c r="AE61" s="15"/>
       <c r="AF61" s="15"/>
       <c r="AG61" s="15"/>
@@ -6621,7 +6766,7 @@
       <c r="AJ61" s="15"/>
       <c r="AK61" s="15"/>
     </row>
-    <row r="62" spans="1:37" ht="127.5">
+    <row r="62" spans="1:37" ht="112.5">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -6672,8 +6817,8 @@
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
       <c r="AB62" s="5"/>
-      <c r="AC62" s="15"/>
-      <c r="AD62" s="15"/>
+      <c r="AC62" s="5"/>
+      <c r="AD62" s="5"/>
       <c r="AE62" s="15"/>
       <c r="AF62" s="15"/>
       <c r="AG62" s="15"/>
@@ -6682,7 +6827,7 @@
       <c r="AJ62" s="15"/>
       <c r="AK62" s="15"/>
     </row>
-    <row r="63" spans="1:37" ht="51">
+    <row r="63" spans="1:37" ht="50">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -6731,8 +6876,8 @@
       <c r="Z63" s="5"/>
       <c r="AA63" s="5"/>
       <c r="AB63" s="5"/>
-      <c r="AC63" s="15"/>
-      <c r="AD63" s="15"/>
+      <c r="AC63" s="5"/>
+      <c r="AD63" s="5"/>
       <c r="AE63" s="15"/>
       <c r="AF63" s="15"/>
       <c r="AG63" s="15"/>
@@ -6741,7 +6886,7 @@
       <c r="AJ63" s="15"/>
       <c r="AK63" s="15"/>
     </row>
-    <row r="64" spans="1:37" ht="76.5">
+    <row r="64" spans="1:37" ht="75">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -6790,8 +6935,10 @@
       <c r="Z64" s="16"/>
       <c r="AA64" s="16"/>
       <c r="AB64" s="16"/>
-    </row>
-    <row r="65" spans="1:37" ht="51">
+      <c r="AC64" s="16"/>
+      <c r="AD64" s="16"/>
+    </row>
+    <row r="65" spans="1:37" ht="50">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -6840,8 +6987,10 @@
       <c r="Z65" s="16"/>
       <c r="AA65" s="16"/>
       <c r="AB65" s="16"/>
-    </row>
-    <row r="66" spans="1:37" ht="63.75">
+      <c r="AC65" s="16"/>
+      <c r="AD65" s="16"/>
+    </row>
+    <row r="66" spans="1:37" ht="62.5">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -6890,8 +7039,10 @@
       <c r="Z66" s="16"/>
       <c r="AA66" s="16"/>
       <c r="AB66" s="16"/>
-    </row>
-    <row r="67" spans="1:37" ht="89.25">
+      <c r="AC66" s="16"/>
+      <c r="AD66" s="16"/>
+    </row>
+    <row r="67" spans="1:37" ht="87.5">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -6940,8 +7091,10 @@
       <c r="Z67" s="16"/>
       <c r="AA67" s="16"/>
       <c r="AB67" s="16"/>
-    </row>
-    <row r="68" spans="1:37" ht="102">
+      <c r="AC67" s="16"/>
+      <c r="AD67" s="16"/>
+    </row>
+    <row r="68" spans="1:37" ht="100">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -6990,8 +7143,10 @@
       <c r="Z68" s="16"/>
       <c r="AA68" s="16"/>
       <c r="AB68" s="16"/>
-    </row>
-    <row r="69" spans="1:37" ht="63.75">
+      <c r="AC68" s="16"/>
+      <c r="AD68" s="16"/>
+    </row>
+    <row r="69" spans="1:37" ht="62.5">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -7040,8 +7195,10 @@
       <c r="Z69" s="16"/>
       <c r="AA69" s="16"/>
       <c r="AB69" s="16"/>
-    </row>
-    <row r="70" spans="1:37" ht="76.5">
+      <c r="AC69" s="16"/>
+      <c r="AD69" s="16"/>
+    </row>
+    <row r="70" spans="1:37" ht="75">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -7090,8 +7247,10 @@
       <c r="Z70" s="16"/>
       <c r="AA70" s="16"/>
       <c r="AB70" s="16"/>
-    </row>
-    <row r="71" spans="1:37" ht="76.5">
+      <c r="AC70" s="16"/>
+      <c r="AD70" s="16"/>
+    </row>
+    <row r="71" spans="1:37" ht="75">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -7140,8 +7299,10 @@
       <c r="Z71" s="16"/>
       <c r="AA71" s="16"/>
       <c r="AB71" s="16"/>
-    </row>
-    <row r="72" spans="1:37" ht="38.25">
+      <c r="AC71" s="16"/>
+      <c r="AD71" s="16"/>
+    </row>
+    <row r="72" spans="1:37" ht="37.5">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -7194,8 +7355,8 @@
       <c r="Z72" s="2"/>
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
-      <c r="AC72" s="14"/>
-      <c r="AD72" s="14"/>
+      <c r="AC72" s="2"/>
+      <c r="AD72" s="2"/>
       <c r="AE72" s="14"/>
       <c r="AF72" s="14"/>
       <c r="AG72" s="14"/>
@@ -7204,7 +7365,7 @@
       <c r="AJ72" s="14"/>
       <c r="AK72" s="14"/>
     </row>
-    <row r="73" spans="1:37" ht="38.25">
+    <row r="73" spans="1:37" ht="25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -7257,8 +7418,8 @@
       <c r="Z73" s="2"/>
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
-      <c r="AC73" s="14"/>
-      <c r="AD73" s="14"/>
+      <c r="AC73" s="2"/>
+      <c r="AD73" s="2"/>
       <c r="AE73" s="14"/>
       <c r="AF73" s="14"/>
       <c r="AG73" s="14"/>
@@ -7267,7 +7428,7 @@
       <c r="AJ73" s="14"/>
       <c r="AK73" s="14"/>
     </row>
-    <row r="74" spans="1:37" ht="38.25">
+    <row r="74" spans="1:37" ht="37.5">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -7320,8 +7481,8 @@
       <c r="Z74" s="2"/>
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
-      <c r="AC74" s="14"/>
-      <c r="AD74" s="14"/>
+      <c r="AC74" s="2"/>
+      <c r="AD74" s="2"/>
       <c r="AE74" s="14"/>
       <c r="AF74" s="14"/>
       <c r="AG74" s="14"/>
@@ -7330,7 +7491,7 @@
       <c r="AJ74" s="14"/>
       <c r="AK74" s="14"/>
     </row>
-    <row r="75" spans="1:37" ht="25.5">
+    <row r="75" spans="1:37" ht="25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -7381,8 +7542,8 @@
       <c r="Z75" s="2"/>
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
-      <c r="AC75" s="14"/>
-      <c r="AD75" s="14"/>
+      <c r="AC75" s="2"/>
+      <c r="AD75" s="2"/>
       <c r="AE75" s="14"/>
       <c r="AF75" s="14"/>
       <c r="AG75" s="14"/>
@@ -7391,7 +7552,7 @@
       <c r="AJ75" s="14"/>
       <c r="AK75" s="14"/>
     </row>
-    <row r="76" spans="1:37" ht="38.25">
+    <row r="76" spans="1:37" ht="37.5">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -7444,8 +7605,8 @@
       <c r="Z76" s="2"/>
       <c r="AA76" s="2"/>
       <c r="AB76" s="2"/>
-      <c r="AC76" s="14"/>
-      <c r="AD76" s="14"/>
+      <c r="AC76" s="2"/>
+      <c r="AD76" s="2"/>
       <c r="AE76" s="14"/>
       <c r="AF76" s="14"/>
       <c r="AG76" s="14"/>
@@ -7454,7 +7615,7 @@
       <c r="AJ76" s="14"/>
       <c r="AK76" s="14"/>
     </row>
-    <row r="77" spans="1:37" ht="38.25">
+    <row r="77" spans="1:37" ht="37.5">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -7507,8 +7668,8 @@
       <c r="Z77" s="2"/>
       <c r="AA77" s="2"/>
       <c r="AB77" s="2"/>
-      <c r="AC77" s="14"/>
-      <c r="AD77" s="14"/>
+      <c r="AC77" s="2"/>
+      <c r="AD77" s="2"/>
       <c r="AE77" s="14"/>
       <c r="AF77" s="14"/>
       <c r="AG77" s="14"/>
@@ -7517,7 +7678,7 @@
       <c r="AJ77" s="14"/>
       <c r="AK77" s="14"/>
     </row>
-    <row r="78" spans="1:37" ht="63.75">
+    <row r="78" spans="1:37" ht="50">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -7570,8 +7731,8 @@
       <c r="Z78" s="2"/>
       <c r="AA78" s="2"/>
       <c r="AB78" s="2"/>
-      <c r="AC78" s="14"/>
-      <c r="AD78" s="14"/>
+      <c r="AC78" s="2"/>
+      <c r="AD78" s="2"/>
       <c r="AE78" s="14"/>
       <c r="AF78" s="14"/>
       <c r="AG78" s="14"/>
@@ -7580,7 +7741,7 @@
       <c r="AJ78" s="14"/>
       <c r="AK78" s="14"/>
     </row>
-    <row r="79" spans="1:37" ht="38.25">
+    <row r="79" spans="1:37" ht="25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -7633,8 +7794,8 @@
       <c r="Z79" s="2"/>
       <c r="AA79" s="2"/>
       <c r="AB79" s="2"/>
-      <c r="AC79" s="14"/>
-      <c r="AD79" s="14"/>
+      <c r="AC79" s="2"/>
+      <c r="AD79" s="2"/>
       <c r="AE79" s="14"/>
       <c r="AF79" s="14"/>
       <c r="AG79" s="14"/>
@@ -7643,7 +7804,7 @@
       <c r="AJ79" s="14"/>
       <c r="AK79" s="14"/>
     </row>
-    <row r="80" spans="1:37" ht="38.25">
+    <row r="80" spans="1:37" ht="25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -7696,8 +7857,8 @@
       <c r="Z80" s="2"/>
       <c r="AA80" s="2"/>
       <c r="AB80" s="2"/>
-      <c r="AC80" s="14"/>
-      <c r="AD80" s="14"/>
+      <c r="AC80" s="2"/>
+      <c r="AD80" s="2"/>
       <c r="AE80" s="14"/>
       <c r="AF80" s="14"/>
       <c r="AG80" s="14"/>
@@ -7706,7 +7867,7 @@
       <c r="AJ80" s="14"/>
       <c r="AK80" s="14"/>
     </row>
-    <row r="81" spans="1:37" ht="25.5">
+    <row r="81" spans="1:37" ht="25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -7759,8 +7920,8 @@
       <c r="Z81" s="2"/>
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
-      <c r="AC81" s="14"/>
-      <c r="AD81" s="14"/>
+      <c r="AC81" s="2"/>
+      <c r="AD81" s="2"/>
       <c r="AE81" s="14"/>
       <c r="AF81" s="14"/>
       <c r="AG81" s="14"/>
@@ -7769,7 +7930,7 @@
       <c r="AJ81" s="14"/>
       <c r="AK81" s="14"/>
     </row>
-    <row r="82" spans="1:37" ht="38.25">
+    <row r="82" spans="1:37" ht="37.5">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -7822,8 +7983,8 @@
       <c r="Z82" s="2"/>
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
-      <c r="AC82" s="14"/>
-      <c r="AD82" s="14"/>
+      <c r="AC82" s="2"/>
+      <c r="AD82" s="2"/>
       <c r="AE82" s="14"/>
       <c r="AF82" s="14"/>
       <c r="AG82" s="14"/>
@@ -7832,7 +7993,7 @@
       <c r="AJ82" s="14"/>
       <c r="AK82" s="14"/>
     </row>
-    <row r="83" spans="1:37" ht="51">
+    <row r="83" spans="1:37" ht="50">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -7885,8 +8046,8 @@
       <c r="Z83" s="2"/>
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
-      <c r="AC83" s="14"/>
-      <c r="AD83" s="14"/>
+      <c r="AC83" s="2"/>
+      <c r="AD83" s="2"/>
       <c r="AE83" s="14"/>
       <c r="AF83" s="14"/>
       <c r="AG83" s="14"/>
@@ -7895,7 +8056,7 @@
       <c r="AJ83" s="14"/>
       <c r="AK83" s="14"/>
     </row>
-    <row r="84" spans="1:37" ht="63.75">
+    <row r="84" spans="1:37" ht="62.5">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -7948,8 +8109,8 @@
       <c r="Z84" s="2"/>
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
-      <c r="AC84" s="14"/>
-      <c r="AD84" s="14"/>
+      <c r="AC84" s="2"/>
+      <c r="AD84" s="2"/>
       <c r="AE84" s="14"/>
       <c r="AF84" s="14"/>
       <c r="AG84" s="14"/>
@@ -7958,7 +8119,7 @@
       <c r="AJ84" s="14"/>
       <c r="AK84" s="14"/>
     </row>
-    <row r="85" spans="1:37" ht="38.25">
+    <row r="85" spans="1:37" ht="37.5">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -8011,8 +8172,8 @@
       <c r="Z85" s="2"/>
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
-      <c r="AC85" s="14"/>
-      <c r="AD85" s="14"/>
+      <c r="AC85" s="2"/>
+      <c r="AD85" s="2"/>
       <c r="AE85" s="14"/>
       <c r="AF85" s="14"/>
       <c r="AG85" s="14"/>
@@ -8021,7 +8182,7 @@
       <c r="AJ85" s="14"/>
       <c r="AK85" s="14"/>
     </row>
-    <row r="86" spans="1:37" ht="51">
+    <row r="86" spans="1:37" ht="37.5">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -8074,8 +8235,8 @@
       <c r="Z86" s="2"/>
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
-      <c r="AC86" s="14"/>
-      <c r="AD86" s="14"/>
+      <c r="AC86" s="2"/>
+      <c r="AD86" s="2"/>
       <c r="AE86" s="14"/>
       <c r="AF86" s="14"/>
       <c r="AG86" s="14"/>
@@ -8084,7 +8245,7 @@
       <c r="AJ86" s="14"/>
       <c r="AK86" s="14"/>
     </row>
-    <row r="87" spans="1:37" ht="76.5">
+    <row r="87" spans="1:37" ht="75">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -8137,8 +8298,8 @@
       <c r="Z87" s="2"/>
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
-      <c r="AC87" s="14"/>
-      <c r="AD87" s="14"/>
+      <c r="AC87" s="2"/>
+      <c r="AD87" s="2"/>
       <c r="AE87" s="14"/>
       <c r="AF87" s="14"/>
       <c r="AG87" s="14"/>
@@ -8147,7 +8308,7 @@
       <c r="AJ87" s="14"/>
       <c r="AK87" s="14"/>
     </row>
-    <row r="88" spans="1:37" ht="51">
+    <row r="88" spans="1:37" ht="50">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -8200,8 +8361,8 @@
       <c r="Z88" s="2"/>
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
-      <c r="AC88" s="14"/>
-      <c r="AD88" s="14"/>
+      <c r="AC88" s="2"/>
+      <c r="AD88" s="2"/>
       <c r="AE88" s="14"/>
       <c r="AF88" s="14"/>
       <c r="AG88" s="14"/>
@@ -8210,7 +8371,7 @@
       <c r="AJ88" s="14"/>
       <c r="AK88" s="14"/>
     </row>
-    <row r="89" spans="1:37" ht="25.5">
+    <row r="89" spans="1:37" ht="25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -8263,8 +8424,8 @@
       <c r="Z89" s="2"/>
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
-      <c r="AC89" s="14"/>
-      <c r="AD89" s="14"/>
+      <c r="AC89" s="2"/>
+      <c r="AD89" s="2"/>
       <c r="AE89" s="14"/>
       <c r="AF89" s="14"/>
       <c r="AG89" s="14"/>
@@ -8273,7 +8434,7 @@
       <c r="AJ89" s="14"/>
       <c r="AK89" s="14"/>
     </row>
-    <row r="90" spans="1:37" ht="51">
+    <row r="90" spans="1:37" ht="50">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -8326,8 +8487,8 @@
       <c r="Z90" s="2"/>
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
-      <c r="AC90" s="14"/>
-      <c r="AD90" s="14"/>
+      <c r="AC90" s="2"/>
+      <c r="AD90" s="2"/>
       <c r="AE90" s="14"/>
       <c r="AF90" s="14"/>
       <c r="AG90" s="14"/>
@@ -8336,7 +8497,7 @@
       <c r="AJ90" s="14"/>
       <c r="AK90" s="14"/>
     </row>
-    <row r="91" spans="1:37" ht="38.25">
+    <row r="91" spans="1:37" ht="37.5">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -8389,8 +8550,8 @@
       <c r="Z91" s="2"/>
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
-      <c r="AC91" s="14"/>
-      <c r="AD91" s="14"/>
+      <c r="AC91" s="2"/>
+      <c r="AD91" s="2"/>
       <c r="AE91" s="14"/>
       <c r="AF91" s="14"/>
       <c r="AG91" s="14"/>
@@ -8399,7 +8560,7 @@
       <c r="AJ91" s="14"/>
       <c r="AK91" s="14"/>
     </row>
-    <row r="92" spans="1:37" ht="38.25">
+    <row r="92" spans="1:37" ht="37.5">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -8448,8 +8609,10 @@
       <c r="Z92" s="16"/>
       <c r="AA92" s="16"/>
       <c r="AB92" s="16"/>
-    </row>
-    <row r="93" spans="1:37" ht="114.75">
+      <c r="AC92" s="16"/>
+      <c r="AD92" s="16"/>
+    </row>
+    <row r="93" spans="1:37" ht="112.5">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -8498,8 +8661,10 @@
       <c r="Z93" s="16"/>
       <c r="AA93" s="16"/>
       <c r="AB93" s="16"/>
-    </row>
-    <row r="94" spans="1:37" ht="38.25">
+      <c r="AC93" s="16"/>
+      <c r="AD93" s="16"/>
+    </row>
+    <row r="94" spans="1:37" ht="37.5">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -8548,8 +8713,10 @@
       <c r="Z94" s="16"/>
       <c r="AA94" s="16"/>
       <c r="AB94" s="16"/>
-    </row>
-    <row r="95" spans="1:37" ht="51">
+      <c r="AC94" s="16"/>
+      <c r="AD94" s="16"/>
+    </row>
+    <row r="95" spans="1:37" ht="50">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -8598,8 +8765,10 @@
       <c r="Z95" s="16"/>
       <c r="AA95" s="16"/>
       <c r="AB95" s="16"/>
-    </row>
-    <row r="96" spans="1:37" ht="51">
+      <c r="AC95" s="16"/>
+      <c r="AD95" s="16"/>
+    </row>
+    <row r="96" spans="1:37" ht="50">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -8648,8 +8817,10 @@
       <c r="Z96" s="16"/>
       <c r="AA96" s="16"/>
       <c r="AB96" s="16"/>
-    </row>
-    <row r="97" spans="1:28" ht="63.75">
+      <c r="AC96" s="16"/>
+      <c r="AD96" s="16"/>
+    </row>
+    <row r="97" spans="1:30" ht="62.5">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -8698,8 +8869,10 @@
       <c r="Z97" s="16"/>
       <c r="AA97" s="16"/>
       <c r="AB97" s="16"/>
-    </row>
-    <row r="98" spans="1:28" ht="89.25">
+      <c r="AC97" s="16"/>
+      <c r="AD97" s="16"/>
+    </row>
+    <row r="98" spans="1:30" ht="75">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -8748,8 +8921,10 @@
       <c r="Z98" s="16"/>
       <c r="AA98" s="16"/>
       <c r="AB98" s="16"/>
-    </row>
-    <row r="99" spans="1:28" ht="38.25">
+      <c r="AC98" s="16"/>
+      <c r="AD98" s="16"/>
+    </row>
+    <row r="99" spans="1:30" ht="37.5">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -8798,8 +8973,10 @@
       <c r="Z99" s="16"/>
       <c r="AA99" s="16"/>
       <c r="AB99" s="16"/>
-    </row>
-    <row r="100" spans="1:28" ht="51">
+      <c r="AC99" s="16"/>
+      <c r="AD99" s="16"/>
+    </row>
+    <row r="100" spans="1:30" ht="50">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -8848,8 +9025,10 @@
       <c r="Z100" s="16"/>
       <c r="AA100" s="16"/>
       <c r="AB100" s="16"/>
-    </row>
-    <row r="101" spans="1:28" ht="63.75">
+      <c r="AC100" s="16"/>
+      <c r="AD100" s="16"/>
+    </row>
+    <row r="101" spans="1:30" ht="62.5">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -8898,8 +9077,10 @@
       <c r="Z101" s="16"/>
       <c r="AA101" s="16"/>
       <c r="AB101" s="16"/>
-    </row>
-    <row r="102" spans="1:28">
+      <c r="AC101" s="16"/>
+      <c r="AD101" s="16"/>
+    </row>
+    <row r="102" spans="1:30">
       <c r="A102" s="14"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
@@ -8911,7 +9092,7 @@
       <c r="L102" s="12"/>
       <c r="O102" s="12"/>
     </row>
-    <row r="103" spans="1:28">
+    <row r="103" spans="1:30">
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
@@ -8922,7 +9103,7 @@
       <c r="L103" s="12"/>
       <c r="O103" s="12"/>
     </row>
-    <row r="104" spans="1:28">
+    <row r="104" spans="1:30">
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -8933,7 +9114,7 @@
       <c r="L104" s="12"/>
       <c r="O104" s="12"/>
     </row>
-    <row r="105" spans="1:28">
+    <row r="105" spans="1:30">
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
@@ -8944,7 +9125,7 @@
       <c r="L105" s="12"/>
       <c r="O105" s="12"/>
     </row>
-    <row r="106" spans="1:28">
+    <row r="106" spans="1:30">
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
@@ -8955,7 +9136,7 @@
       <c r="L106" s="12"/>
       <c r="O106" s="12"/>
     </row>
-    <row r="107" spans="1:28">
+    <row r="107" spans="1:30">
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
@@ -8966,7 +9147,7 @@
       <c r="L107" s="12"/>
       <c r="O107" s="12"/>
     </row>
-    <row r="108" spans="1:28">
+    <row r="108" spans="1:30">
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
@@ -8977,7 +9158,7 @@
       <c r="L108" s="12"/>
       <c r="O108" s="12"/>
     </row>
-    <row r="109" spans="1:28">
+    <row r="109" spans="1:30">
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
@@ -8988,7 +9169,7 @@
       <c r="L109" s="12"/>
       <c r="O109" s="12"/>
     </row>
-    <row r="110" spans="1:28">
+    <row r="110" spans="1:30">
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -8999,7 +9180,7 @@
       <c r="L110" s="12"/>
       <c r="O110" s="12"/>
     </row>
-    <row r="111" spans="1:28">
+    <row r="111" spans="1:30">
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
@@ -9010,7 +9191,7 @@
       <c r="L111" s="12"/>
       <c r="O111" s="12"/>
     </row>
-    <row r="112" spans="1:28">
+    <row r="112" spans="1:30">
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>

</xml_diff>

<commit_message>
Initial commit 03-12-2025  1:38:04.02
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEDAE9A-2C39-493A-B109-07994DC6E82F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A90419E-E008-4654-818B-EDDC0366749D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3209,8 +3209,8 @@
   </sheetPr>
   <dimension ref="A1:AK999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
Initial commit 05-12-2025 12:59:51.77
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A90419E-E008-4654-818B-EDDC0366749D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3670339-5154-45F5-976D-6C0032B83696}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="640">
   <si>
     <t>Sl No</t>
   </si>
@@ -2831,6 +2831,12 @@
   </si>
   <si>
     <t>Regional Language (Malayalam)</t>
+  </si>
+  <si>
+    <t>Negative Marks/Question</t>
+  </si>
+  <si>
+    <t>Marks/Question</t>
   </si>
 </sst>
 </file>
@@ -3210,7 +3216,7 @@
   <dimension ref="A1:AK999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="A1:XFD1048576"/>
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5"/>
@@ -3313,6 +3319,12 @@
       <c r="AD1" s="1" t="s">
         <v>626</v>
       </c>
+      <c r="AE1" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="2" spans="1:37" ht="287.5">
       <c r="A2" s="2">
@@ -3381,8 +3393,12 @@
       <c r="AD2" s="2">
         <v>0.75</v>
       </c>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
+      <c r="AE2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0.66</v>
+      </c>
       <c r="AG2" s="14"/>
       <c r="AH2" s="14"/>
       <c r="AI2" s="14"/>
@@ -3454,8 +3470,8 @@
         <v>628</v>
       </c>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
       <c r="AG3" s="14"/>
       <c r="AH3" s="14"/>
       <c r="AI3" s="14"/>
@@ -3529,8 +3545,8 @@
         <v>629</v>
       </c>
       <c r="AD4" s="2"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
       <c r="AG4" s="14"/>
       <c r="AH4" s="14"/>
       <c r="AI4" s="14"/>
@@ -3602,8 +3618,8 @@
         <v>630</v>
       </c>
       <c r="AD5" s="2"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
       <c r="AG5" s="14"/>
       <c r="AH5" s="14"/>
       <c r="AI5" s="14"/>
@@ -3675,8 +3691,8 @@
         <v>631</v>
       </c>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
       <c r="AG6" s="14"/>
       <c r="AH6" s="14"/>
       <c r="AI6" s="14"/>
@@ -3748,8 +3764,8 @@
         <v>632</v>
       </c>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
       <c r="AG7" s="14"/>
       <c r="AH7" s="14"/>
       <c r="AI7" s="14"/>
@@ -3821,8 +3837,8 @@
         <v>633</v>
       </c>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
       <c r="AG8" s="14"/>
       <c r="AH8" s="14"/>
       <c r="AI8" s="14"/>
@@ -3894,8 +3910,8 @@
         <v>634</v>
       </c>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
       <c r="AG9" s="14"/>
       <c r="AH9" s="14"/>
       <c r="AI9" s="14"/>
@@ -3967,8 +3983,8 @@
         <v>635</v>
       </c>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
       <c r="AG10" s="14"/>
       <c r="AH10" s="14"/>
       <c r="AI10" s="14"/>
@@ -4042,8 +4058,8 @@
         <v>636</v>
       </c>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
       <c r="AG11" s="14"/>
       <c r="AH11" s="14"/>
       <c r="AI11" s="14"/>
@@ -4109,8 +4125,8 @@
         <v>637</v>
       </c>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
       <c r="AG12" s="14"/>
       <c r="AH12" s="14"/>
       <c r="AI12" s="14"/>
@@ -4170,8 +4186,8 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="15"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
       <c r="AG13" s="15"/>
       <c r="AH13" s="15"/>
       <c r="AI13" s="15"/>
@@ -4231,6 +4247,8 @@
       <c r="AB14" s="16"/>
       <c r="AC14" s="16"/>
       <c r="AD14" s="16"/>
+      <c r="AE14" s="16"/>
+      <c r="AF14" s="16"/>
     </row>
     <row r="15" spans="1:37" ht="350">
       <c r="A15" s="2">
@@ -4283,6 +4301,8 @@
       <c r="AB15" s="16"/>
       <c r="AC15" s="16"/>
       <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
     </row>
     <row r="16" spans="1:37" ht="350">
       <c r="A16" s="2">
@@ -4335,8 +4355,10 @@
       <c r="AB16" s="16"/>
       <c r="AC16" s="16"/>
       <c r="AD16" s="16"/>
-    </row>
-    <row r="17" spans="1:30" ht="375">
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="16"/>
+    </row>
+    <row r="17" spans="1:32" ht="375">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4387,8 +4409,10 @@
       <c r="AB17" s="16"/>
       <c r="AC17" s="16"/>
       <c r="AD17" s="16"/>
-    </row>
-    <row r="18" spans="1:30" ht="409.5">
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="16"/>
+    </row>
+    <row r="18" spans="1:32" ht="409.5">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -4439,8 +4463,10 @@
       <c r="AB18" s="16"/>
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
-    </row>
-    <row r="19" spans="1:30" ht="409.5">
+      <c r="AE18" s="16"/>
+      <c r="AF18" s="16"/>
+    </row>
+    <row r="19" spans="1:32" ht="409.5">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4491,8 +4517,10 @@
       <c r="AB19" s="16"/>
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
-    </row>
-    <row r="20" spans="1:30" ht="409.5">
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+    </row>
+    <row r="20" spans="1:32" ht="409.5">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4543,8 +4571,10 @@
       <c r="AB20" s="16"/>
       <c r="AC20" s="16"/>
       <c r="AD20" s="16"/>
-    </row>
-    <row r="21" spans="1:30" ht="409.5">
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+    </row>
+    <row r="21" spans="1:32" ht="409.5">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4595,8 +4625,10 @@
       <c r="AB21" s="16"/>
       <c r="AC21" s="16"/>
       <c r="AD21" s="16"/>
-    </row>
-    <row r="22" spans="1:30" ht="409.5">
+      <c r="AE21" s="16"/>
+      <c r="AF21" s="16"/>
+    </row>
+    <row r="22" spans="1:32" ht="409.5">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -4647,8 +4679,10 @@
       <c r="AB22" s="16"/>
       <c r="AC22" s="16"/>
       <c r="AD22" s="16"/>
-    </row>
-    <row r="23" spans="1:30" ht="409.5">
+      <c r="AE22" s="16"/>
+      <c r="AF22" s="16"/>
+    </row>
+    <row r="23" spans="1:32" ht="409.5">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -4699,8 +4733,10 @@
       <c r="AB23" s="16"/>
       <c r="AC23" s="16"/>
       <c r="AD23" s="16"/>
-    </row>
-    <row r="24" spans="1:30" ht="409.5">
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="16"/>
+    </row>
+    <row r="24" spans="1:32" ht="409.5">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -4751,8 +4787,10 @@
       <c r="AB24" s="16"/>
       <c r="AC24" s="16"/>
       <c r="AD24" s="16"/>
-    </row>
-    <row r="25" spans="1:30" ht="409.5">
+      <c r="AE24" s="16"/>
+      <c r="AF24" s="16"/>
+    </row>
+    <row r="25" spans="1:32" ht="409.5">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -4803,8 +4841,10 @@
       <c r="AB25" s="16"/>
       <c r="AC25" s="16"/>
       <c r="AD25" s="16"/>
-    </row>
-    <row r="26" spans="1:30" ht="375">
+      <c r="AE25" s="16"/>
+      <c r="AF25" s="16"/>
+    </row>
+    <row r="26" spans="1:32" ht="375">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -4855,8 +4895,10 @@
       <c r="AB26" s="16"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="16"/>
-    </row>
-    <row r="27" spans="1:30" ht="350">
+      <c r="AE26" s="16"/>
+      <c r="AF26" s="16"/>
+    </row>
+    <row r="27" spans="1:32" ht="350">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4907,8 +4949,10 @@
       <c r="AB27" s="16"/>
       <c r="AC27" s="16"/>
       <c r="AD27" s="16"/>
-    </row>
-    <row r="28" spans="1:30" ht="409.5">
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+    </row>
+    <row r="28" spans="1:32" ht="409.5">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -4959,8 +5003,10 @@
       <c r="AB28" s="16"/>
       <c r="AC28" s="16"/>
       <c r="AD28" s="16"/>
-    </row>
-    <row r="29" spans="1:30" ht="409.5">
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="16"/>
+    </row>
+    <row r="29" spans="1:32" ht="409.5">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5011,8 +5057,10 @@
       <c r="AB29" s="16"/>
       <c r="AC29" s="16"/>
       <c r="AD29" s="16"/>
-    </row>
-    <row r="30" spans="1:30" ht="409.5">
+      <c r="AE29" s="16"/>
+      <c r="AF29" s="16"/>
+    </row>
+    <row r="30" spans="1:32" ht="409.5">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5063,8 +5111,10 @@
       <c r="AB30" s="16"/>
       <c r="AC30" s="16"/>
       <c r="AD30" s="16"/>
-    </row>
-    <row r="31" spans="1:30" ht="409.5">
+      <c r="AE30" s="16"/>
+      <c r="AF30" s="16"/>
+    </row>
+    <row r="31" spans="1:32" ht="409.5">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5115,8 +5165,10 @@
       <c r="AB31" s="16"/>
       <c r="AC31" s="16"/>
       <c r="AD31" s="16"/>
-    </row>
-    <row r="32" spans="1:30" ht="409.5">
+      <c r="AE31" s="16"/>
+      <c r="AF31" s="16"/>
+    </row>
+    <row r="32" spans="1:32" ht="409.5">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5167,8 +5219,10 @@
       <c r="AB32" s="16"/>
       <c r="AC32" s="16"/>
       <c r="AD32" s="16"/>
-    </row>
-    <row r="33" spans="1:30" ht="409.5">
+      <c r="AE32" s="16"/>
+      <c r="AF32" s="16"/>
+    </row>
+    <row r="33" spans="1:32" ht="409.5">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5219,8 +5273,10 @@
       <c r="AB33" s="16"/>
       <c r="AC33" s="16"/>
       <c r="AD33" s="16"/>
-    </row>
-    <row r="34" spans="1:30" ht="300">
+      <c r="AE33" s="16"/>
+      <c r="AF33" s="16"/>
+    </row>
+    <row r="34" spans="1:32" ht="300">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5271,8 +5327,10 @@
       <c r="AB34" s="16"/>
       <c r="AC34" s="16"/>
       <c r="AD34" s="16"/>
-    </row>
-    <row r="35" spans="1:30" ht="175">
+      <c r="AE34" s="16"/>
+      <c r="AF34" s="16"/>
+    </row>
+    <row r="35" spans="1:32" ht="175">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5323,8 +5381,10 @@
       <c r="AB35" s="16"/>
       <c r="AC35" s="16"/>
       <c r="AD35" s="16"/>
-    </row>
-    <row r="36" spans="1:30" ht="312.5">
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+    </row>
+    <row r="36" spans="1:32" ht="312.5">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5375,8 +5435,10 @@
       <c r="AB36" s="16"/>
       <c r="AC36" s="16"/>
       <c r="AD36" s="16"/>
-    </row>
-    <row r="37" spans="1:30" ht="237.5">
+      <c r="AE36" s="16"/>
+      <c r="AF36" s="16"/>
+    </row>
+    <row r="37" spans="1:32" ht="237.5">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5427,8 +5489,10 @@
       <c r="AB37" s="16"/>
       <c r="AC37" s="16"/>
       <c r="AD37" s="16"/>
-    </row>
-    <row r="38" spans="1:30" ht="137.5">
+      <c r="AE37" s="16"/>
+      <c r="AF37" s="16"/>
+    </row>
+    <row r="38" spans="1:32" ht="137.5">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5479,8 +5543,10 @@
       <c r="AB38" s="16"/>
       <c r="AC38" s="16"/>
       <c r="AD38" s="16"/>
-    </row>
-    <row r="39" spans="1:30" ht="237.5">
+      <c r="AE38" s="16"/>
+      <c r="AF38" s="16"/>
+    </row>
+    <row r="39" spans="1:32" ht="237.5">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5531,8 +5597,10 @@
       <c r="AB39" s="16"/>
       <c r="AC39" s="16"/>
       <c r="AD39" s="16"/>
-    </row>
-    <row r="40" spans="1:30" ht="225">
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="16"/>
+    </row>
+    <row r="40" spans="1:32" ht="225">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5583,8 +5651,10 @@
       <c r="AB40" s="16"/>
       <c r="AC40" s="16"/>
       <c r="AD40" s="16"/>
-    </row>
-    <row r="41" spans="1:30" ht="150">
+      <c r="AE40" s="16"/>
+      <c r="AF40" s="16"/>
+    </row>
+    <row r="41" spans="1:32" ht="150">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5635,8 +5705,10 @@
       <c r="AB41" s="16"/>
       <c r="AC41" s="16"/>
       <c r="AD41" s="16"/>
-    </row>
-    <row r="42" spans="1:30" ht="337.5">
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+    </row>
+    <row r="42" spans="1:32" ht="337.5">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -5687,8 +5759,10 @@
       <c r="AB42" s="16"/>
       <c r="AC42" s="16"/>
       <c r="AD42" s="16"/>
-    </row>
-    <row r="43" spans="1:30" ht="150">
+      <c r="AE42" s="16"/>
+      <c r="AF42" s="16"/>
+    </row>
+    <row r="43" spans="1:32" ht="150">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5739,8 +5813,10 @@
       <c r="AB43" s="16"/>
       <c r="AC43" s="16"/>
       <c r="AD43" s="16"/>
-    </row>
-    <row r="44" spans="1:30" ht="350">
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+    </row>
+    <row r="44" spans="1:32" ht="350">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -5791,8 +5867,10 @@
       <c r="AB44" s="16"/>
       <c r="AC44" s="16"/>
       <c r="AD44" s="16"/>
-    </row>
-    <row r="45" spans="1:30" ht="262.5">
+      <c r="AE44" s="16"/>
+      <c r="AF44" s="16"/>
+    </row>
+    <row r="45" spans="1:32" ht="262.5">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5843,8 +5921,10 @@
       <c r="AB45" s="16"/>
       <c r="AC45" s="16"/>
       <c r="AD45" s="16"/>
-    </row>
-    <row r="46" spans="1:30" ht="187.5">
+      <c r="AE45" s="16"/>
+      <c r="AF45" s="16"/>
+    </row>
+    <row r="46" spans="1:32" ht="187.5">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -5895,8 +5975,10 @@
       <c r="AB46" s="16"/>
       <c r="AC46" s="16"/>
       <c r="AD46" s="16"/>
-    </row>
-    <row r="47" spans="1:30" ht="409.5">
+      <c r="AE46" s="16"/>
+      <c r="AF46" s="16"/>
+    </row>
+    <row r="47" spans="1:32" ht="409.5">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -5947,8 +6029,10 @@
       <c r="AB47" s="16"/>
       <c r="AC47" s="16"/>
       <c r="AD47" s="16"/>
-    </row>
-    <row r="48" spans="1:30" ht="375">
+      <c r="AE47" s="16"/>
+      <c r="AF47" s="16"/>
+    </row>
+    <row r="48" spans="1:32" ht="375">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -5999,6 +6083,8 @@
       <c r="AB48" s="16"/>
       <c r="AC48" s="16"/>
       <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
     </row>
     <row r="49" spans="1:37" ht="409.5">
       <c r="A49" s="2">
@@ -6051,6 +6137,8 @@
       <c r="AB49" s="16"/>
       <c r="AC49" s="16"/>
       <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
     </row>
     <row r="50" spans="1:37" ht="312.5">
       <c r="A50" s="2">
@@ -6103,6 +6191,8 @@
       <c r="AB50" s="16"/>
       <c r="AC50" s="16"/>
       <c r="AD50" s="16"/>
+      <c r="AE50" s="16"/>
+      <c r="AF50" s="16"/>
     </row>
     <row r="51" spans="1:37" ht="409.5">
       <c r="A51" s="2">
@@ -6155,6 +6245,8 @@
       <c r="AB51" s="16"/>
       <c r="AC51" s="16"/>
       <c r="AD51" s="16"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
     </row>
     <row r="52" spans="1:37" ht="300">
       <c r="A52" s="2">
@@ -6209,8 +6301,8 @@
       <c r="AB52" s="5"/>
       <c r="AC52" s="5"/>
       <c r="AD52" s="5"/>
-      <c r="AE52" s="15"/>
-      <c r="AF52" s="15"/>
+      <c r="AE52" s="5"/>
+      <c r="AF52" s="5"/>
       <c r="AG52" s="15"/>
       <c r="AH52" s="15"/>
       <c r="AI52" s="15"/>
@@ -6270,8 +6362,8 @@
       <c r="AB53" s="5"/>
       <c r="AC53" s="5"/>
       <c r="AD53" s="5"/>
-      <c r="AE53" s="15"/>
-      <c r="AF53" s="15"/>
+      <c r="AE53" s="5"/>
+      <c r="AF53" s="5"/>
       <c r="AG53" s="15"/>
       <c r="AH53" s="15"/>
       <c r="AI53" s="15"/>
@@ -6331,8 +6423,8 @@
       <c r="AB54" s="5"/>
       <c r="AC54" s="5"/>
       <c r="AD54" s="5"/>
-      <c r="AE54" s="15"/>
-      <c r="AF54" s="15"/>
+      <c r="AE54" s="5"/>
+      <c r="AF54" s="5"/>
       <c r="AG54" s="15"/>
       <c r="AH54" s="15"/>
       <c r="AI54" s="15"/>
@@ -6392,8 +6484,8 @@
       <c r="AB55" s="5"/>
       <c r="AC55" s="5"/>
       <c r="AD55" s="5"/>
-      <c r="AE55" s="15"/>
-      <c r="AF55" s="15"/>
+      <c r="AE55" s="5"/>
+      <c r="AF55" s="5"/>
       <c r="AG55" s="15"/>
       <c r="AH55" s="15"/>
       <c r="AI55" s="15"/>
@@ -6453,8 +6545,8 @@
       <c r="AB56" s="5"/>
       <c r="AC56" s="5"/>
       <c r="AD56" s="5"/>
-      <c r="AE56" s="15"/>
-      <c r="AF56" s="15"/>
+      <c r="AE56" s="5"/>
+      <c r="AF56" s="5"/>
       <c r="AG56" s="15"/>
       <c r="AH56" s="15"/>
       <c r="AI56" s="15"/>
@@ -6514,8 +6606,8 @@
       <c r="AB57" s="5"/>
       <c r="AC57" s="5"/>
       <c r="AD57" s="5"/>
-      <c r="AE57" s="15"/>
-      <c r="AF57" s="15"/>
+      <c r="AE57" s="5"/>
+      <c r="AF57" s="5"/>
       <c r="AG57" s="15"/>
       <c r="AH57" s="15"/>
       <c r="AI57" s="15"/>
@@ -6575,8 +6667,8 @@
       <c r="AB58" s="5"/>
       <c r="AC58" s="5"/>
       <c r="AD58" s="5"/>
-      <c r="AE58" s="15"/>
-      <c r="AF58" s="15"/>
+      <c r="AE58" s="5"/>
+      <c r="AF58" s="5"/>
       <c r="AG58" s="15"/>
       <c r="AH58" s="15"/>
       <c r="AI58" s="15"/>
@@ -6636,8 +6728,8 @@
       <c r="AB59" s="5"/>
       <c r="AC59" s="5"/>
       <c r="AD59" s="5"/>
-      <c r="AE59" s="15"/>
-      <c r="AF59" s="15"/>
+      <c r="AE59" s="5"/>
+      <c r="AF59" s="5"/>
       <c r="AG59" s="15"/>
       <c r="AH59" s="15"/>
       <c r="AI59" s="15"/>
@@ -6697,8 +6789,8 @@
       <c r="AB60" s="5"/>
       <c r="AC60" s="5"/>
       <c r="AD60" s="5"/>
-      <c r="AE60" s="15"/>
-      <c r="AF60" s="15"/>
+      <c r="AE60" s="5"/>
+      <c r="AF60" s="5"/>
       <c r="AG60" s="15"/>
       <c r="AH60" s="15"/>
       <c r="AI60" s="15"/>
@@ -6758,8 +6850,8 @@
       <c r="AB61" s="5"/>
       <c r="AC61" s="5"/>
       <c r="AD61" s="5"/>
-      <c r="AE61" s="15"/>
-      <c r="AF61" s="15"/>
+      <c r="AE61" s="5"/>
+      <c r="AF61" s="5"/>
       <c r="AG61" s="15"/>
       <c r="AH61" s="15"/>
       <c r="AI61" s="15"/>
@@ -6819,8 +6911,8 @@
       <c r="AB62" s="5"/>
       <c r="AC62" s="5"/>
       <c r="AD62" s="5"/>
-      <c r="AE62" s="15"/>
-      <c r="AF62" s="15"/>
+      <c r="AE62" s="5"/>
+      <c r="AF62" s="5"/>
       <c r="AG62" s="15"/>
       <c r="AH62" s="15"/>
       <c r="AI62" s="15"/>
@@ -6878,8 +6970,8 @@
       <c r="AB63" s="5"/>
       <c r="AC63" s="5"/>
       <c r="AD63" s="5"/>
-      <c r="AE63" s="15"/>
-      <c r="AF63" s="15"/>
+      <c r="AE63" s="5"/>
+      <c r="AF63" s="5"/>
       <c r="AG63" s="15"/>
       <c r="AH63" s="15"/>
       <c r="AI63" s="15"/>
@@ -6937,6 +7029,8 @@
       <c r="AB64" s="16"/>
       <c r="AC64" s="16"/>
       <c r="AD64" s="16"/>
+      <c r="AE64" s="16"/>
+      <c r="AF64" s="16"/>
     </row>
     <row r="65" spans="1:37" ht="50">
       <c r="A65" s="2">
@@ -6989,6 +7083,8 @@
       <c r="AB65" s="16"/>
       <c r="AC65" s="16"/>
       <c r="AD65" s="16"/>
+      <c r="AE65" s="16"/>
+      <c r="AF65" s="16"/>
     </row>
     <row r="66" spans="1:37" ht="62.5">
       <c r="A66" s="2">
@@ -7041,6 +7137,8 @@
       <c r="AB66" s="16"/>
       <c r="AC66" s="16"/>
       <c r="AD66" s="16"/>
+      <c r="AE66" s="16"/>
+      <c r="AF66" s="16"/>
     </row>
     <row r="67" spans="1:37" ht="87.5">
       <c r="A67" s="2">
@@ -7093,6 +7191,8 @@
       <c r="AB67" s="16"/>
       <c r="AC67" s="16"/>
       <c r="AD67" s="16"/>
+      <c r="AE67" s="16"/>
+      <c r="AF67" s="16"/>
     </row>
     <row r="68" spans="1:37" ht="100">
       <c r="A68" s="2">
@@ -7145,6 +7245,8 @@
       <c r="AB68" s="16"/>
       <c r="AC68" s="16"/>
       <c r="AD68" s="16"/>
+      <c r="AE68" s="16"/>
+      <c r="AF68" s="16"/>
     </row>
     <row r="69" spans="1:37" ht="62.5">
       <c r="A69" s="2">
@@ -7197,6 +7299,8 @@
       <c r="AB69" s="16"/>
       <c r="AC69" s="16"/>
       <c r="AD69" s="16"/>
+      <c r="AE69" s="16"/>
+      <c r="AF69" s="16"/>
     </row>
     <row r="70" spans="1:37" ht="75">
       <c r="A70" s="2">
@@ -7249,6 +7353,8 @@
       <c r="AB70" s="16"/>
       <c r="AC70" s="16"/>
       <c r="AD70" s="16"/>
+      <c r="AE70" s="16"/>
+      <c r="AF70" s="16"/>
     </row>
     <row r="71" spans="1:37" ht="75">
       <c r="A71" s="2">
@@ -7301,6 +7407,8 @@
       <c r="AB71" s="16"/>
       <c r="AC71" s="16"/>
       <c r="AD71" s="16"/>
+      <c r="AE71" s="16"/>
+      <c r="AF71" s="16"/>
     </row>
     <row r="72" spans="1:37" ht="37.5">
       <c r="A72" s="2">
@@ -7357,8 +7465,8 @@
       <c r="AB72" s="2"/>
       <c r="AC72" s="2"/>
       <c r="AD72" s="2"/>
-      <c r="AE72" s="14"/>
-      <c r="AF72" s="14"/>
+      <c r="AE72" s="2"/>
+      <c r="AF72" s="2"/>
       <c r="AG72" s="14"/>
       <c r="AH72" s="14"/>
       <c r="AI72" s="14"/>
@@ -7420,8 +7528,8 @@
       <c r="AB73" s="2"/>
       <c r="AC73" s="2"/>
       <c r="AD73" s="2"/>
-      <c r="AE73" s="14"/>
-      <c r="AF73" s="14"/>
+      <c r="AE73" s="2"/>
+      <c r="AF73" s="2"/>
       <c r="AG73" s="14"/>
       <c r="AH73" s="14"/>
       <c r="AI73" s="14"/>
@@ -7483,8 +7591,8 @@
       <c r="AB74" s="2"/>
       <c r="AC74" s="2"/>
       <c r="AD74" s="2"/>
-      <c r="AE74" s="14"/>
-      <c r="AF74" s="14"/>
+      <c r="AE74" s="2"/>
+      <c r="AF74" s="2"/>
       <c r="AG74" s="14"/>
       <c r="AH74" s="14"/>
       <c r="AI74" s="14"/>
@@ -7544,8 +7652,8 @@
       <c r="AB75" s="2"/>
       <c r="AC75" s="2"/>
       <c r="AD75" s="2"/>
-      <c r="AE75" s="14"/>
-      <c r="AF75" s="14"/>
+      <c r="AE75" s="2"/>
+      <c r="AF75" s="2"/>
       <c r="AG75" s="14"/>
       <c r="AH75" s="14"/>
       <c r="AI75" s="14"/>
@@ -7607,8 +7715,8 @@
       <c r="AB76" s="2"/>
       <c r="AC76" s="2"/>
       <c r="AD76" s="2"/>
-      <c r="AE76" s="14"/>
-      <c r="AF76" s="14"/>
+      <c r="AE76" s="2"/>
+      <c r="AF76" s="2"/>
       <c r="AG76" s="14"/>
       <c r="AH76" s="14"/>
       <c r="AI76" s="14"/>
@@ -7670,8 +7778,8 @@
       <c r="AB77" s="2"/>
       <c r="AC77" s="2"/>
       <c r="AD77" s="2"/>
-      <c r="AE77" s="14"/>
-      <c r="AF77" s="14"/>
+      <c r="AE77" s="2"/>
+      <c r="AF77" s="2"/>
       <c r="AG77" s="14"/>
       <c r="AH77" s="14"/>
       <c r="AI77" s="14"/>
@@ -7733,8 +7841,8 @@
       <c r="AB78" s="2"/>
       <c r="AC78" s="2"/>
       <c r="AD78" s="2"/>
-      <c r="AE78" s="14"/>
-      <c r="AF78" s="14"/>
+      <c r="AE78" s="2"/>
+      <c r="AF78" s="2"/>
       <c r="AG78" s="14"/>
       <c r="AH78" s="14"/>
       <c r="AI78" s="14"/>
@@ -7796,8 +7904,8 @@
       <c r="AB79" s="2"/>
       <c r="AC79" s="2"/>
       <c r="AD79" s="2"/>
-      <c r="AE79" s="14"/>
-      <c r="AF79" s="14"/>
+      <c r="AE79" s="2"/>
+      <c r="AF79" s="2"/>
       <c r="AG79" s="14"/>
       <c r="AH79" s="14"/>
       <c r="AI79" s="14"/>
@@ -7859,8 +7967,8 @@
       <c r="AB80" s="2"/>
       <c r="AC80" s="2"/>
       <c r="AD80" s="2"/>
-      <c r="AE80" s="14"/>
-      <c r="AF80" s="14"/>
+      <c r="AE80" s="2"/>
+      <c r="AF80" s="2"/>
       <c r="AG80" s="14"/>
       <c r="AH80" s="14"/>
       <c r="AI80" s="14"/>
@@ -7922,8 +8030,8 @@
       <c r="AB81" s="2"/>
       <c r="AC81" s="2"/>
       <c r="AD81" s="2"/>
-      <c r="AE81" s="14"/>
-      <c r="AF81" s="14"/>
+      <c r="AE81" s="2"/>
+      <c r="AF81" s="2"/>
       <c r="AG81" s="14"/>
       <c r="AH81" s="14"/>
       <c r="AI81" s="14"/>
@@ -7985,8 +8093,8 @@
       <c r="AB82" s="2"/>
       <c r="AC82" s="2"/>
       <c r="AD82" s="2"/>
-      <c r="AE82" s="14"/>
-      <c r="AF82" s="14"/>
+      <c r="AE82" s="2"/>
+      <c r="AF82" s="2"/>
       <c r="AG82" s="14"/>
       <c r="AH82" s="14"/>
       <c r="AI82" s="14"/>
@@ -8048,8 +8156,8 @@
       <c r="AB83" s="2"/>
       <c r="AC83" s="2"/>
       <c r="AD83" s="2"/>
-      <c r="AE83" s="14"/>
-      <c r="AF83" s="14"/>
+      <c r="AE83" s="2"/>
+      <c r="AF83" s="2"/>
       <c r="AG83" s="14"/>
       <c r="AH83" s="14"/>
       <c r="AI83" s="14"/>
@@ -8111,8 +8219,8 @@
       <c r="AB84" s="2"/>
       <c r="AC84" s="2"/>
       <c r="AD84" s="2"/>
-      <c r="AE84" s="14"/>
-      <c r="AF84" s="14"/>
+      <c r="AE84" s="2"/>
+      <c r="AF84" s="2"/>
       <c r="AG84" s="14"/>
       <c r="AH84" s="14"/>
       <c r="AI84" s="14"/>
@@ -8174,8 +8282,8 @@
       <c r="AB85" s="2"/>
       <c r="AC85" s="2"/>
       <c r="AD85" s="2"/>
-      <c r="AE85" s="14"/>
-      <c r="AF85" s="14"/>
+      <c r="AE85" s="2"/>
+      <c r="AF85" s="2"/>
       <c r="AG85" s="14"/>
       <c r="AH85" s="14"/>
       <c r="AI85" s="14"/>
@@ -8237,8 +8345,8 @@
       <c r="AB86" s="2"/>
       <c r="AC86" s="2"/>
       <c r="AD86" s="2"/>
-      <c r="AE86" s="14"/>
-      <c r="AF86" s="14"/>
+      <c r="AE86" s="2"/>
+      <c r="AF86" s="2"/>
       <c r="AG86" s="14"/>
       <c r="AH86" s="14"/>
       <c r="AI86" s="14"/>
@@ -8300,8 +8408,8 @@
       <c r="AB87" s="2"/>
       <c r="AC87" s="2"/>
       <c r="AD87" s="2"/>
-      <c r="AE87" s="14"/>
-      <c r="AF87" s="14"/>
+      <c r="AE87" s="2"/>
+      <c r="AF87" s="2"/>
       <c r="AG87" s="14"/>
       <c r="AH87" s="14"/>
       <c r="AI87" s="14"/>
@@ -8363,8 +8471,8 @@
       <c r="AB88" s="2"/>
       <c r="AC88" s="2"/>
       <c r="AD88" s="2"/>
-      <c r="AE88" s="14"/>
-      <c r="AF88" s="14"/>
+      <c r="AE88" s="2"/>
+      <c r="AF88" s="2"/>
       <c r="AG88" s="14"/>
       <c r="AH88" s="14"/>
       <c r="AI88" s="14"/>
@@ -8426,8 +8534,8 @@
       <c r="AB89" s="2"/>
       <c r="AC89" s="2"/>
       <c r="AD89" s="2"/>
-      <c r="AE89" s="14"/>
-      <c r="AF89" s="14"/>
+      <c r="AE89" s="2"/>
+      <c r="AF89" s="2"/>
       <c r="AG89" s="14"/>
       <c r="AH89" s="14"/>
       <c r="AI89" s="14"/>
@@ -8489,8 +8597,8 @@
       <c r="AB90" s="2"/>
       <c r="AC90" s="2"/>
       <c r="AD90" s="2"/>
-      <c r="AE90" s="14"/>
-      <c r="AF90" s="14"/>
+      <c r="AE90" s="2"/>
+      <c r="AF90" s="2"/>
       <c r="AG90" s="14"/>
       <c r="AH90" s="14"/>
       <c r="AI90" s="14"/>
@@ -8552,8 +8660,8 @@
       <c r="AB91" s="2"/>
       <c r="AC91" s="2"/>
       <c r="AD91" s="2"/>
-      <c r="AE91" s="14"/>
-      <c r="AF91" s="14"/>
+      <c r="AE91" s="2"/>
+      <c r="AF91" s="2"/>
       <c r="AG91" s="14"/>
       <c r="AH91" s="14"/>
       <c r="AI91" s="14"/>
@@ -8611,6 +8719,8 @@
       <c r="AB92" s="16"/>
       <c r="AC92" s="16"/>
       <c r="AD92" s="16"/>
+      <c r="AE92" s="16"/>
+      <c r="AF92" s="16"/>
     </row>
     <row r="93" spans="1:37" ht="112.5">
       <c r="A93" s="2">
@@ -8663,6 +8773,8 @@
       <c r="AB93" s="16"/>
       <c r="AC93" s="16"/>
       <c r="AD93" s="16"/>
+      <c r="AE93" s="16"/>
+      <c r="AF93" s="16"/>
     </row>
     <row r="94" spans="1:37" ht="37.5">
       <c r="A94" s="2">
@@ -8715,6 +8827,8 @@
       <c r="AB94" s="16"/>
       <c r="AC94" s="16"/>
       <c r="AD94" s="16"/>
+      <c r="AE94" s="16"/>
+      <c r="AF94" s="16"/>
     </row>
     <row r="95" spans="1:37" ht="50">
       <c r="A95" s="2">
@@ -8767,6 +8881,8 @@
       <c r="AB95" s="16"/>
       <c r="AC95" s="16"/>
       <c r="AD95" s="16"/>
+      <c r="AE95" s="16"/>
+      <c r="AF95" s="16"/>
     </row>
     <row r="96" spans="1:37" ht="50">
       <c r="A96" s="2">
@@ -8819,8 +8935,10 @@
       <c r="AB96" s="16"/>
       <c r="AC96" s="16"/>
       <c r="AD96" s="16"/>
-    </row>
-    <row r="97" spans="1:30" ht="62.5">
+      <c r="AE96" s="16"/>
+      <c r="AF96" s="16"/>
+    </row>
+    <row r="97" spans="1:32" ht="62.5">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -8871,8 +8989,10 @@
       <c r="AB97" s="16"/>
       <c r="AC97" s="16"/>
       <c r="AD97" s="16"/>
-    </row>
-    <row r="98" spans="1:30" ht="75">
+      <c r="AE97" s="16"/>
+      <c r="AF97" s="16"/>
+    </row>
+    <row r="98" spans="1:32" ht="75">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -8923,8 +9043,10 @@
       <c r="AB98" s="16"/>
       <c r="AC98" s="16"/>
       <c r="AD98" s="16"/>
-    </row>
-    <row r="99" spans="1:30" ht="37.5">
+      <c r="AE98" s="16"/>
+      <c r="AF98" s="16"/>
+    </row>
+    <row r="99" spans="1:32" ht="37.5">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -8975,8 +9097,10 @@
       <c r="AB99" s="16"/>
       <c r="AC99" s="16"/>
       <c r="AD99" s="16"/>
-    </row>
-    <row r="100" spans="1:30" ht="50">
+      <c r="AE99" s="16"/>
+      <c r="AF99" s="16"/>
+    </row>
+    <row r="100" spans="1:32" ht="50">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -9027,8 +9151,10 @@
       <c r="AB100" s="16"/>
       <c r="AC100" s="16"/>
       <c r="AD100" s="16"/>
-    </row>
-    <row r="101" spans="1:30" ht="62.5">
+      <c r="AE100" s="16"/>
+      <c r="AF100" s="16"/>
+    </row>
+    <row r="101" spans="1:32" ht="62.5">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -9079,8 +9205,10 @@
       <c r="AB101" s="16"/>
       <c r="AC101" s="16"/>
       <c r="AD101" s="16"/>
-    </row>
-    <row r="102" spans="1:30">
+      <c r="AE101" s="16"/>
+      <c r="AF101" s="16"/>
+    </row>
+    <row r="102" spans="1:32">
       <c r="A102" s="14"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
@@ -9092,7 +9220,7 @@
       <c r="L102" s="12"/>
       <c r="O102" s="12"/>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:32">
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
@@ -9103,7 +9231,7 @@
       <c r="L103" s="12"/>
       <c r="O103" s="12"/>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:32">
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -9114,7 +9242,7 @@
       <c r="L104" s="12"/>
       <c r="O104" s="12"/>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:32">
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
@@ -9125,7 +9253,7 @@
       <c r="L105" s="12"/>
       <c r="O105" s="12"/>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:32">
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
@@ -9136,7 +9264,7 @@
       <c r="L106" s="12"/>
       <c r="O106" s="12"/>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:32">
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
@@ -9147,7 +9275,7 @@
       <c r="L107" s="12"/>
       <c r="O107" s="12"/>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:32">
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
@@ -9158,7 +9286,7 @@
       <c r="L108" s="12"/>
       <c r="O108" s="12"/>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:32">
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
@@ -9169,7 +9297,7 @@
       <c r="L109" s="12"/>
       <c r="O109" s="12"/>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:32">
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -9180,7 +9308,7 @@
       <c r="L110" s="12"/>
       <c r="O110" s="12"/>
     </row>
-    <row r="111" spans="1:30">
+    <row r="111" spans="1:32">
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
@@ -9191,7 +9319,7 @@
       <c r="L111" s="12"/>
       <c r="O111" s="12"/>
     </row>
-    <row r="112" spans="1:30">
+    <row r="112" spans="1:32">
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>

</xml_diff>

<commit_message>
Initial commit 05-12-2025 13:30:55.53
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7DCDD1-04D0-42F8-A8E8-C2AED13123DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ACEA70-35B8-490A-9411-5E7D5F22DBF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3238,8 +3238,8 @@
   </sheetPr>
   <dimension ref="A1:AQ999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
Initial commit 05-12-2025 14:15:37.13
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ACEA70-35B8-490A-9411-5E7D5F22DBF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F397615-6C82-49BD-AE36-7E8E131ABF56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3238,8 +3238,8 @@
   </sheetPr>
   <dimension ref="A1:AQ999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5"/>
@@ -3455,10 +3455,10 @@
         <v>0.75</v>
       </c>
       <c r="AK2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL2" s="2">
-        <v>0.66</v>
+        <v>0.33</v>
       </c>
       <c r="AM2" s="14"/>
       <c r="AN2" s="14"/>

</xml_diff>

<commit_message>
Initial commit 11-12-2025 20:11:24.50
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E502ECC-4810-4486-AA96-D77310DA375B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D4EA5-F9F1-44D0-9E63-5652C4DD61A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3592,7 +3592,7 @@
     <t>Question Image</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP/view?usp=sharing</t>
+    <t>https://drive.google.com/uc?**export=view&amp;id**=1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</t>
   </si>
 </sst>
 </file>
@@ -3771,9 +3771,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4001,7 +3999,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -53200,8 +53198,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{6D2F88E6-5060-4DC9-BC1E-BD66A7EED7B9}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{D4B74CA9-BFEC-412C-B998-EC6C77C79F4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit 11-12-2025 20:16:26.40
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D4EA5-F9F1-44D0-9E63-5652C4DD61A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06235692-3CC3-4CF3-8089-2F0F560045E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="909">
   <si>
     <t>Sl No</t>
   </si>
@@ -3592,7 +3592,7 @@
     <t>Question Image</t>
   </si>
   <si>
-    <t>https://drive.google.com/uc?**export=view&amp;id**=1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</t>
+    <t>https://drive.google.com/uc?export=view&amp;id=1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</t>
   </si>
 </sst>
 </file>
@@ -4288,7 +4288,9 @@
       <c r="R3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="5"/>
+      <c r="S3" s="21" t="s">
+        <v>908</v>
+      </c>
       <c r="T3" s="5" t="s">
         <v>48</v>
       </c>
@@ -53198,9 +53200,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{D4B74CA9-BFEC-412C-B998-EC6C77C79F4C}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{7A41D3B9-B40B-49D0-B64F-78FB81C1E98B}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{71A9D80A-FA05-4DE9-8BD7-91E3F2C63141}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit 11-12-2025 20:20:43.58
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06235692-3CC3-4CF3-8089-2F0F560045E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFC2E73-4AE4-4FC3-BEA8-8ADD1E842C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="910">
   <si>
     <t>Sl No</t>
   </si>
@@ -3593,6 +3593,9 @@
   </si>
   <si>
     <t>https://drive.google.com/uc?export=view&amp;id=1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/d/1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</t>
   </si>
 </sst>
 </file>
@@ -4188,7 +4191,7 @@
         <v>47</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Initial commit 11-12-2025 20:47:59.10
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C8E267-086E-4131-9F4D-E2F9D03E50A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0504E8CE-93F3-4059-AA04-A9DED3C44A26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="910">
   <si>
     <t>Sl No</t>
   </si>
@@ -4037,9 +4037,9 @@
   </sheetPr>
   <dimension ref="A1:AS999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ3" sqref="AJ3"/>
+      <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4338,7 +4338,9 @@
       <c r="R3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="5"/>
+      <c r="S3" s="23" t="s">
+        <v>909</v>
+      </c>
       <c r="T3" s="5" t="s">
         <v>48</v>
       </c>
@@ -4368,8 +4370,8 @@
       <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="21" t="str">
-        <f>IF(S3="","",CONCATENATE("https://lh3.googleusercontent.com/d/",S3))</f>
-        <v/>
+        <f t="shared" ref="AJ3:AJ6" si="0">IF(S3="","",CONCATENATE("https://lh3.googleusercontent.com/d/",S3))</f>
+        <v>https://lh3.googleusercontent.com/d/1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</v>
       </c>
       <c r="AK3" s="5" t="s">
         <v>65</v>
@@ -4465,7 +4467,10 @@
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
+      <c r="AJ4" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="AK4" s="5" t="s">
         <v>79</v>
       </c>
@@ -4557,7 +4562,10 @@
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
+      <c r="AJ5" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="AK5" s="5" t="s">
         <v>89</v>
       </c>
@@ -4650,7 +4658,10 @@
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
+      <c r="AJ6" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="AK6" s="5" t="s">
         <v>101</v>
       </c>
@@ -54249,7 +54260,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AJ2" r:id="rId1" display="https://lh3.googleusercontent.com/d/1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP" xr:uid="{7A41D3B9-B40B-49D0-B64F-78FB81C1E98B}"/>
-    <hyperlink ref="AJ3" r:id="rId2" display="https://lh3.googleusercontent.com/d/1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP" xr:uid="{888DE7F2-3387-4146-9BAA-55981C41C6B0}"/>
+    <hyperlink ref="AJ3:AJ6" r:id="rId2" display="https://lh3.googleusercontent.com/d/1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP" xr:uid="{CC22BA12-E87A-4CB0-A4A8-605E647BB77A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Initial commit 11-12-2025 20:57:57.59
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0504E8CE-93F3-4059-AA04-A9DED3C44A26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F03EEF-76C3-496D-B23F-179BA4319309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="911">
   <si>
     <t>Sl No</t>
   </si>
@@ -3596,6 +3596,9 @@
   </si>
   <si>
     <t>1guCfI26c3wGc_RxfSOnRSwcEvP2XThtP</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -4037,9 +4040,9 @@
   </sheetPr>
   <dimension ref="A1:AS999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
+      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4438,7 +4441,9 @@
       <c r="R4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="S4" s="23" t="s">
+        <v>910</v>
+      </c>
       <c r="T4" s="5" t="s">
         <v>48</v>
       </c>
@@ -4469,7 +4474,7 @@
       <c r="AI4" s="5"/>
       <c r="AJ4" s="21" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>https://lh3.googleusercontent.com/d/NA</v>
       </c>
       <c r="AK4" s="5" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Initial commit 11-12-2025 21:48:23.84
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEFEA9A-27DC-4B60-B348-D8B23E54B727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E04EBD7-8D74-474C-AFD6-9EC8D88829A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3598,9 +3598,6 @@
     <t>Google Drive Image ID_Question</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=ibw3-fIrgbY</t>
-  </si>
-  <si>
     <t>Explanation Video</t>
   </si>
   <si>
@@ -3608,6 +3605,9 @@
   </si>
   <si>
     <t>Google Drive Image ID_Explanatiom</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=EngW7tLk6R8</t>
   </si>
 </sst>
 </file>
@@ -4046,9 +4046,9 @@
   </sheetPr>
   <dimension ref="A1:AV999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM9" sqref="AM9"/>
+      <selection pane="bottomLeft" activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4128,10 +4128,10 @@
         <v>909</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>18</v>
@@ -4185,7 +4185,7 @@
         <v>907</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>34</v>
@@ -4263,7 +4263,7 @@
         <v>908</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Initial commit 11-12-2025 22:13:21.68
</commit_message>
<xml_diff>
--- a/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
+++ b/Question_Data_Folder/KPSC/Mock Test/Degree Level/Degree Prelims/QB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manup\Desktop\projectk\Question_Data_Folder\KPSC\Mock Test\Degree Level\Degree Prelims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E04EBD7-8D74-474C-AFD6-9EC8D88829A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1789623A-B68B-41C8-A333-6F4529B99236}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3598,7 +3598,7 @@
     <t>Google Drive Image ID_Question</t>
   </si>
   <si>
-    <t>Explanation Video</t>
+    <t>Explanation Media</t>
   </si>
   <si>
     <t>Explanation Image</t>
@@ -4048,7 +4048,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U6" sqref="U6"/>
+      <selection pane="bottomLeft" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>